<commit_message>
report RT end? testing
</commit_message>
<xml_diff>
--- a/doc/oil/Маслосклад.xlsx
+++ b/doc/oil/Маслосклад.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2017\Projects\Work\FuelControl\doc\oil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2013\Projects\Work\FuelControl\doc\oil\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,11 +14,12 @@
   <sheets>
     <sheet name="Остатки" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="4" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="5" r:id="rId3"/>
-    <sheet name="Лист1" sheetId="3" r:id="rId4"/>
+    <sheet name="Лист4" sheetId="6" r:id="rId3"/>
+    <sheet name="Лист3" sheetId="5" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Лист1!$B$2:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Лист1!$B$2:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Лист2!$A$1:$E$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Остатки!$B$1:$K$41</definedName>
   </definedNames>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="211">
   <si>
     <t>Timestamp</t>
   </si>
@@ -605,12 +606,72 @@
   </si>
   <si>
     <t>Группа-4 №24</t>
+  </si>
+  <si>
+    <t>Группа-5 №03</t>
+  </si>
+  <si>
+    <t>Группа-5 №06</t>
+  </si>
+  <si>
+    <t>Группа-5 №09</t>
+  </si>
+  <si>
+    <t>Группа-5 №12</t>
+  </si>
+  <si>
+    <t>Группа-5 №15</t>
+  </si>
+  <si>
+    <t>Группа-5 №18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малый бак№1        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малый бак№2        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малый бак№3        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малый бак№4        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малый бак№5        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №1        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №2        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №3        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №4        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №5        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филиал №6        </t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>); break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> : return(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -985,7 +1046,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
@@ -1024,24 +1085,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1096,6 +1139,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Вывод" xfId="4" builtinId="21"/>
@@ -1471,7 +1533,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="67" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3">
@@ -1506,7 +1568,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="67"/>
       <c r="B3" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1539,7 +1601,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1572,7 +1634,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1605,7 +1667,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1638,7 +1700,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1671,7 +1733,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="8">
         <v>43626.602268518516</v>
       </c>
@@ -1704,7 +1766,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="64" t="s">
         <v>134</v>
       </c>
       <c r="B9" s="14">
@@ -1739,7 +1801,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -1772,7 +1834,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -1805,7 +1867,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -1838,7 +1900,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="16">
         <v>43626.602268518516</v>
       </c>
@@ -1871,7 +1933,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="18">
         <v>43626.602268518516</v>
       </c>
@@ -1904,7 +1966,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="67" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="6">
@@ -1939,7 +2001,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -1972,7 +2034,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2005,7 +2067,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="21">
         <v>43626.602268518516</v>
       </c>
@@ -2038,7 +2100,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="67" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="3">
@@ -2073,7 +2135,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2106,7 +2168,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2139,7 +2201,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2172,7 +2234,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2205,7 +2267,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
+      <c r="A24" s="67"/>
       <c r="B24" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2238,7 +2300,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2271,7 +2333,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="21">
         <v>43626.602268518516</v>
       </c>
@@ -2304,7 +2366,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="67" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="3">
@@ -2339,7 +2401,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="67"/>
       <c r="B28" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2372,7 +2434,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="67"/>
       <c r="B29" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2405,7 +2467,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="41"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="21">
         <v>43626.602268518516</v>
       </c>
@@ -2438,7 +2500,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="67" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3">
@@ -2473,7 +2535,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2506,7 +2568,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="24">
         <v>43626.602268518516</v>
       </c>
@@ -2539,7 +2601,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="67"/>
       <c r="B34" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2572,7 +2634,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="67"/>
       <c r="B35" s="6">
         <v>43626.602268518516</v>
       </c>
@@ -2605,7 +2667,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
+      <c r="A36" s="67"/>
       <c r="B36" s="21">
         <v>43626.602268518516</v>
       </c>
@@ -2638,7 +2700,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="62" t="s">
         <v>125</v>
       </c>
       <c r="B37" s="14">
@@ -2673,7 +2735,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="37"/>
+      <c r="A38" s="63"/>
       <c r="B38" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -2706,7 +2768,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -2739,7 +2801,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="37"/>
+      <c r="A40" s="63"/>
       <c r="B40" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -2772,7 +2834,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
+      <c r="A41" s="63"/>
       <c r="B41" s="12">
         <v>43626.602268518516</v>
       </c>
@@ -2824,13 +2886,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65:E78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
@@ -2864,7 +2927,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="36">
         <v>1</v>
       </c>
       <c r="D2" t="s">
@@ -2884,7 +2947,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="36">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -2904,7 +2967,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="36">
         <v>3</v>
       </c>
       <c r="D4" t="s">
@@ -2924,7 +2987,7 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="36">
         <v>4</v>
       </c>
       <c r="D5" t="s">
@@ -2944,7 +3007,7 @@
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="36">
         <v>6</v>
       </c>
       <c r="D6" t="s">
@@ -2964,7 +3027,7 @@
       <c r="B7">
         <v>35</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="36">
         <v>35</v>
       </c>
       <c r="D7" t="s">
@@ -2978,1160 +3041,1160 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
+      <c r="A8" s="39">
         <v>4</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="40">
         <v>132</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="45">
+      <c r="E8" s="39">
         <v>310008401</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="47">
+      <c r="A9" s="41">
         <v>3</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="42">
         <v>132</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="41">
         <v>310008401</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="41" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="A10" s="41">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="48">
+      <c r="C10" s="42">
         <v>132</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="41">
         <v>310008400</v>
       </c>
-      <c r="F10" s="47" t="s">
+      <c r="F10" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
+      <c r="A11" s="39">
         <v>6</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="40">
         <v>135</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="39">
         <v>310008400</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
+      <c r="A12" s="39">
         <v>7</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="40">
         <v>138</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="39">
         <v>310008401</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="45">
+      <c r="A13" s="39">
         <v>8</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="40">
         <v>139</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="39">
         <v>310008400</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+      <c r="A14" s="39">
         <v>10</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="40">
         <v>141</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="39">
         <v>310008401</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="47">
+      <c r="A15" s="41">
         <v>9</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="42">
         <v>141</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="41">
         <v>310008401</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
+      <c r="A16" s="39">
         <v>12</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="40">
         <v>142</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="39">
         <v>310008400</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="39" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
+      <c r="A17" s="41">
         <v>11</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="42">
         <v>142</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="41">
         <v>310008399</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="41" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="A18" s="39">
         <v>12</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="40">
         <v>144</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="39">
         <v>310008400</v>
       </c>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="39" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="53">
+      <c r="A19" s="47">
         <v>16</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="49">
         <v>225</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="48">
         <v>310008438</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="F19" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="53">
+      <c r="A20" s="47">
         <v>15</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="50">
         <v>225</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="47">
         <v>310008413</v>
       </c>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="47" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
+      <c r="A21" s="47">
         <v>14</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="50">
         <v>225</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="53">
+      <c r="E21" s="47">
         <v>310008438</v>
       </c>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="47" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54" t="s">
+      <c r="A22" s="48"/>
+      <c r="B22" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="C22" s="55">
+      <c r="C22" s="49">
         <v>228</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="48">
         <v>310008438</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="53">
+      <c r="A23" s="47">
         <v>18</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="56">
+      <c r="C23" s="50">
         <v>228</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="53">
+      <c r="E23" s="47">
         <v>310008401</v>
       </c>
-      <c r="F23" s="53" t="s">
+      <c r="F23" s="47" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="53">
+      <c r="A24" s="47">
         <v>17</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="C24" s="56">
+      <c r="C24" s="50">
         <v>228</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E24" s="47">
         <v>310008438</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="47" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25" s="48">
         <v>22</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="49">
         <v>229</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="48">
         <v>310008407</v>
       </c>
-      <c r="F25" s="54" t="s">
+      <c r="F25" s="48" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="53">
+      <c r="A26" s="47">
         <v>21</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="50">
         <v>229</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="E26" s="53">
+      <c r="E26" s="47">
         <v>310008407</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="47" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="53">
+      <c r="A27" s="47">
         <v>20</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="C27" s="56">
+      <c r="C27" s="50">
         <v>229</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D27" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="53">
+      <c r="E27" s="47">
         <v>310008400</v>
       </c>
-      <c r="F27" s="53" t="s">
+      <c r="F27" s="47" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="54">
+      <c r="A28" s="48">
         <v>27</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C28" s="55">
+      <c r="C28" s="49">
         <v>231</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="48">
         <v>310008400</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="48" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="53">
+      <c r="A29" s="47">
         <v>26</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="50">
         <v>231</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="53">
+      <c r="E29" s="47">
         <v>310008400</v>
       </c>
-      <c r="F29" s="53" t="s">
+      <c r="F29" s="47" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="53">
+      <c r="A30" s="47">
         <v>25</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="56">
+      <c r="C30" s="50">
         <v>231</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="53">
+      <c r="E30" s="47">
         <v>310008413</v>
       </c>
-      <c r="F30" s="53" t="s">
+      <c r="F30" s="47" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="53">
+      <c r="A31" s="47">
         <v>24</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="C31" s="56">
+      <c r="C31" s="50">
         <v>231</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D31" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="53">
+      <c r="E31" s="47">
         <v>310008400</v>
       </c>
-      <c r="F31" s="53" t="s">
+      <c r="F31" s="47" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="53">
+      <c r="A32" s="47">
         <v>23</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="56">
+      <c r="C32" s="50">
         <v>231</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D32" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="53">
+      <c r="E32" s="47">
         <v>310008401</v>
       </c>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="47" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="50">
+      <c r="A33" s="44">
         <v>29</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="C33" s="51">
+      <c r="C33" s="45">
         <v>301</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="D33" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="50">
+      <c r="E33" s="44">
         <v>310008413</v>
       </c>
-      <c r="F33" s="50" t="s">
+      <c r="F33" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="50">
+      <c r="A34" s="44">
         <v>30</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="51">
+      <c r="C34" s="45">
         <v>304</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="44">
         <v>310008413</v>
       </c>
-      <c r="F34" s="50" t="s">
+      <c r="F34" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="50">
+      <c r="A35" s="44">
         <v>31</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="C35" s="51">
+      <c r="C35" s="45">
         <v>307</v>
       </c>
-      <c r="D35" s="50" t="s">
+      <c r="D35" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="50">
+      <c r="E35" s="44">
         <v>310008413</v>
       </c>
-      <c r="F35" s="50" t="s">
+      <c r="F35" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="50">
+      <c r="A36" s="44">
         <v>32</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="C36" s="51">
+      <c r="C36" s="45">
         <v>310</v>
       </c>
-      <c r="D36" s="50" t="s">
+      <c r="D36" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="44">
         <v>310008413</v>
       </c>
-      <c r="F36" s="50" t="s">
+      <c r="F36" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="50">
+      <c r="A37" s="44">
         <v>33</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="45">
         <v>313</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="44">
         <v>310008413</v>
       </c>
-      <c r="F37" s="50" t="s">
+      <c r="F37" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="50">
+      <c r="A38" s="44">
         <v>34</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="C38" s="51">
+      <c r="C38" s="45">
         <v>316</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="44">
         <v>310008413</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F38" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="50">
+      <c r="A39" s="44">
         <v>39</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="C39" s="51">
+      <c r="C39" s="45">
         <v>319</v>
       </c>
-      <c r="D39" s="50" t="s">
+      <c r="D39" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="50">
+      <c r="E39" s="44">
         <v>310008407</v>
       </c>
-      <c r="F39" s="50" t="s">
+      <c r="F39" s="44" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="49">
+      <c r="A40" s="43">
         <v>38</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C40" s="52">
+      <c r="C40" s="46">
         <v>319</v>
       </c>
-      <c r="D40" s="49" t="s">
+      <c r="D40" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="49">
+      <c r="E40" s="43">
         <v>310008407</v>
       </c>
-      <c r="F40" s="49" t="s">
+      <c r="F40" s="43" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="49">
+      <c r="A41" s="43">
         <v>37</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="52">
+      <c r="C41" s="46">
         <v>319</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="49">
+      <c r="E41" s="43">
         <v>310008413</v>
       </c>
-      <c r="F41" s="49" t="s">
+      <c r="F41" s="43" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="49">
+      <c r="A42" s="43">
         <v>36</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C42" s="52">
+      <c r="C42" s="46">
         <v>319</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="49">
+      <c r="E42" s="43">
         <v>310038031</v>
       </c>
-      <c r="F42" s="49" t="s">
+      <c r="F42" s="43" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="49">
+      <c r="A43" s="43">
         <v>35</v>
       </c>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="52">
+      <c r="C43" s="46">
         <v>319</v>
       </c>
-      <c r="D43" s="49" t="s">
+      <c r="D43" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="49">
+      <c r="E43" s="43">
         <v>310008413</v>
       </c>
-      <c r="F43" s="49" t="s">
+      <c r="F43" s="43" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="49">
+      <c r="A44" s="43">
         <v>42</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="C44" s="51">
+      <c r="C44" s="45">
         <v>322</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="E44" s="50">
+      <c r="E44" s="44">
         <v>310008413</v>
       </c>
-      <c r="F44" s="50" t="s">
+      <c r="F44" s="44" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="49">
+      <c r="A45" s="43">
         <v>41</v>
       </c>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="C45" s="52">
+      <c r="C45" s="46">
         <v>322</v>
       </c>
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="49">
+      <c r="E45" s="43">
         <v>310008438</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="43" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="49">
+      <c r="A46" s="43">
         <v>40</v>
       </c>
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="46">
         <v>322</v>
       </c>
-      <c r="D46" s="49" t="s">
+      <c r="D46" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="49">
+      <c r="E46" s="43">
         <v>310008413</v>
       </c>
-      <c r="F46" s="49" t="s">
+      <c r="F46" s="43" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="57">
+      <c r="A47" s="51">
         <v>46</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="C47" s="58">
+      <c r="C47" s="52">
         <v>420</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="E47" s="57">
+      <c r="E47" s="51">
         <v>310008398</v>
       </c>
-      <c r="F47" s="57" t="s">
+      <c r="F47" s="51" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="59">
+      <c r="A48" s="53">
         <v>45</v>
       </c>
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="53" t="s">
         <v>187</v>
       </c>
-      <c r="C48" s="60">
+      <c r="C48" s="54">
         <v>420</v>
       </c>
-      <c r="D48" s="59" t="s">
+      <c r="D48" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="59">
+      <c r="E48" s="53">
         <v>310008398</v>
       </c>
-      <c r="F48" s="59" t="s">
+      <c r="F48" s="53" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="57">
+      <c r="A49" s="51">
         <v>48</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="58">
+      <c r="C49" s="52">
         <v>421</v>
       </c>
-      <c r="D49" s="57" t="s">
+      <c r="D49" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="E49" s="57">
+      <c r="E49" s="51">
         <v>310008399</v>
       </c>
-      <c r="F49" s="57" t="s">
+      <c r="F49" s="51" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="59">
+      <c r="A50" s="53">
         <v>47</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="C50" s="60">
+      <c r="C50" s="54">
         <v>421</v>
       </c>
-      <c r="D50" s="59" t="s">
+      <c r="D50" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="E50" s="59">
+      <c r="E50" s="53">
         <v>310008399</v>
       </c>
-      <c r="F50" s="59" t="s">
+      <c r="F50" s="53" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="57">
+      <c r="A51" s="51">
         <v>49</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="C51" s="58">
+      <c r="C51" s="52">
         <v>423</v>
       </c>
-      <c r="D51" s="57" t="s">
+      <c r="D51" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="E51" s="57">
+      <c r="E51" s="51">
         <v>310008399</v>
       </c>
-      <c r="F51" s="57" t="s">
+      <c r="F51" s="51" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="57">
+      <c r="A52" s="51">
         <v>50</v>
       </c>
-      <c r="B52" s="57" t="s">
+      <c r="B52" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="C52" s="58">
+      <c r="C52" s="52">
         <v>424</v>
       </c>
-      <c r="D52" s="57" t="s">
+      <c r="D52" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="E52" s="57">
+      <c r="E52" s="51">
         <v>310008398</v>
       </c>
-      <c r="F52" s="57" t="s">
+      <c r="F52" s="51" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="61">
+      <c r="A53" s="55">
         <v>51</v>
       </c>
-      <c r="B53" s="61">
+      <c r="B53" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="56">
         <v>503</v>
       </c>
-      <c r="C53" s="62">
+      <c r="D53" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="55">
+        <v>310008411</v>
+      </c>
+      <c r="F53" s="55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="55">
+        <v>52</v>
+      </c>
+      <c r="B54" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="C54" s="56">
+        <v>506</v>
+      </c>
+      <c r="D54" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="E54" s="55">
+        <v>310008411</v>
+      </c>
+      <c r="F54" s="55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="55">
+        <v>53</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="56">
+        <v>509</v>
+      </c>
+      <c r="D55" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="55">
+        <v>310008412</v>
+      </c>
+      <c r="F55" s="55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="55">
+        <v>53</v>
+      </c>
+      <c r="B56" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="56">
+        <v>512</v>
+      </c>
+      <c r="D56" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="55">
+        <v>310008412</v>
+      </c>
+      <c r="F56" s="55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="55">
+        <v>54</v>
+      </c>
+      <c r="B57" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="56">
+        <v>515</v>
+      </c>
+      <c r="D57" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E57" s="55">
+        <v>310008412</v>
+      </c>
+      <c r="F57" s="55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="55">
+        <v>51</v>
+      </c>
+      <c r="B58" s="55" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="56">
         <v>503</v>
       </c>
-      <c r="D53" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="E53" s="61">
+      <c r="D58" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" s="55">
         <v>310008411</v>
       </c>
-      <c r="F53" s="61" t="s">
+      <c r="F58" s="55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="61">
-        <v>52</v>
-      </c>
-      <c r="B54" s="61">
-        <v>506</v>
-      </c>
-      <c r="C54" s="62">
-        <v>506</v>
-      </c>
-      <c r="D54" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54" s="61">
-        <v>310008411</v>
-      </c>
-      <c r="F54" s="61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="61">
-        <v>53</v>
-      </c>
-      <c r="B55" s="61">
-        <v>509</v>
-      </c>
-      <c r="C55" s="62">
-        <v>509</v>
-      </c>
-      <c r="D55" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="E55" s="61">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="57">
+        <v>56</v>
+      </c>
+      <c r="B59" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="58">
+        <v>9189</v>
+      </c>
+      <c r="D59" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" s="57">
+        <v>310008401</v>
+      </c>
+      <c r="F59" s="57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="57">
+        <v>57</v>
+      </c>
+      <c r="B60" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="C60" s="58">
+        <v>9190</v>
+      </c>
+      <c r="D60" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="57">
+        <v>310008398</v>
+      </c>
+      <c r="F60" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="57">
+        <v>58</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C61" s="58">
+        <v>9191</v>
+      </c>
+      <c r="D61" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" s="57">
+        <v>310008399</v>
+      </c>
+      <c r="F61" s="57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="57">
+        <v>59</v>
+      </c>
+      <c r="B62" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="58">
+        <v>9192</v>
+      </c>
+      <c r="D62" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="57">
+        <v>310008400</v>
+      </c>
+      <c r="F62" s="57" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="57">
+        <v>61</v>
+      </c>
+      <c r="B63" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="C63" s="58">
+        <v>9193</v>
+      </c>
+      <c r="D63" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E63" s="57">
         <v>310008412</v>
       </c>
-      <c r="F55" s="61" t="s">
+      <c r="F63" s="57" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="61">
-        <v>53</v>
-      </c>
-      <c r="B56" s="61">
-        <v>512</v>
-      </c>
-      <c r="C56" s="62">
-        <v>512</v>
-      </c>
-      <c r="D56" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="E56" s="61">
-        <v>310008412</v>
-      </c>
-      <c r="F56" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="61">
-        <v>54</v>
-      </c>
-      <c r="B57" s="61">
-        <v>515</v>
-      </c>
-      <c r="C57" s="62">
-        <v>515</v>
-      </c>
-      <c r="D57" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="E57" s="61">
-        <v>310008412</v>
-      </c>
-      <c r="F57" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="61">
-        <v>51</v>
-      </c>
-      <c r="B58" s="61">
-        <v>518</v>
-      </c>
-      <c r="C58" s="62">
-        <v>503</v>
-      </c>
-      <c r="D58" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="E58" s="61">
-        <v>310008411</v>
-      </c>
-      <c r="F58" s="61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="63">
-        <v>56</v>
-      </c>
-      <c r="B59" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="C59" s="64">
-        <v>9189</v>
-      </c>
-      <c r="D59" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="E59" s="63">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="59">
+        <v>60</v>
+      </c>
+      <c r="B64" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" s="60">
+        <v>9193</v>
+      </c>
+      <c r="D64" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="E64" s="59">
         <v>310008401</v>
       </c>
-      <c r="F59" s="63" t="s">
+      <c r="F64" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="63">
-        <v>57</v>
-      </c>
-      <c r="B60" s="63" t="s">
-        <v>96</v>
-      </c>
-      <c r="C60" s="64">
-        <v>9190</v>
-      </c>
-      <c r="D60" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="63">
-        <v>310008398</v>
-      </c>
-      <c r="F60" s="63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="63">
-        <v>58</v>
-      </c>
-      <c r="B61" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="C61" s="64">
-        <v>9191</v>
-      </c>
-      <c r="D61" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="E61" s="63">
-        <v>310008399</v>
-      </c>
-      <c r="F61" s="63" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="63">
-        <v>59</v>
-      </c>
-      <c r="B62" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="64">
-        <v>9192</v>
-      </c>
-      <c r="D62" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" s="63">
-        <v>310008400</v>
-      </c>
-      <c r="F62" s="63" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="63">
-        <v>61</v>
-      </c>
-      <c r="B63" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C63" s="64">
-        <v>9193</v>
-      </c>
-      <c r="D63" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="E63" s="63">
-        <v>310008412</v>
-      </c>
-      <c r="F63" s="63" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="65">
-        <v>60</v>
-      </c>
-      <c r="B64" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="66">
-        <v>9193</v>
-      </c>
-      <c r="D64" s="65" t="s">
-        <v>103</v>
-      </c>
-      <c r="E64" s="65">
-        <v>310008401</v>
-      </c>
-      <c r="F64" s="65" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="43">
+      <c r="A65" s="37">
         <v>62</v>
       </c>
-      <c r="B65" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C65" s="44">
+      <c r="B65" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="38">
         <v>195</v>
       </c>
-      <c r="D65" s="43" t="s">
+      <c r="D65" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="43">
+      <c r="E65" s="37">
         <v>310008413</v>
       </c>
-      <c r="F65" s="43" t="s">
+      <c r="F65" s="37" t="s">
         <v>34</v>
       </c>
       <c r="I65">
@@ -4139,22 +4202,22 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="43">
+      <c r="A66" s="37">
         <v>66</v>
       </c>
-      <c r="B66" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="44">
+      <c r="B66" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="C66" s="38">
         <v>196</v>
       </c>
-      <c r="D66" s="43" t="s">
+      <c r="D66" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E66" s="43">
+      <c r="E66" s="37">
         <v>310008413</v>
       </c>
-      <c r="F66" s="43" t="s">
+      <c r="F66" s="37" t="s">
         <v>53</v>
       </c>
       <c r="I66">
@@ -4166,9 +4229,9 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>107</v>
-      </c>
-      <c r="C67" s="67">
+        <v>203</v>
+      </c>
+      <c r="C67" s="61">
         <v>196</v>
       </c>
       <c r="D67" t="s">
@@ -4189,9 +4252,9 @@
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="67">
+        <v>203</v>
+      </c>
+      <c r="C68" s="61">
         <v>196</v>
       </c>
       <c r="D68" t="s">
@@ -4212,9 +4275,9 @@
         <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
-      </c>
-      <c r="C69" s="67">
+        <v>203</v>
+      </c>
+      <c r="C69" s="61">
         <v>196</v>
       </c>
       <c r="D69" t="s">
@@ -4231,22 +4294,22 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="43">
+      <c r="A70" s="37">
         <v>69</v>
       </c>
-      <c r="B70" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C70" s="44">
+      <c r="B70" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" s="38">
         <v>197</v>
       </c>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="E70" s="43">
+      <c r="E70" s="37">
         <v>310008413</v>
       </c>
-      <c r="F70" s="43" t="s">
+      <c r="F70" s="37" t="s">
         <v>53</v>
       </c>
       <c r="I70">
@@ -4258,9 +4321,9 @@
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
-      </c>
-      <c r="C71" s="67">
+        <v>204</v>
+      </c>
+      <c r="C71" s="61">
         <v>197</v>
       </c>
       <c r="D71" t="s">
@@ -4278,9 +4341,9 @@
         <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" s="67">
+        <v>204</v>
+      </c>
+      <c r="C72" s="61">
         <v>197</v>
       </c>
       <c r="D72" t="s">
@@ -4294,22 +4357,22 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="43">
+      <c r="A73" s="37">
         <v>72</v>
       </c>
-      <c r="B73" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="C73" s="44">
+      <c r="B73" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" s="38">
         <v>198</v>
       </c>
-      <c r="D73" s="43" t="s">
+      <c r="D73" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="E73" s="43">
+      <c r="E73" s="37">
         <v>310008413</v>
       </c>
-      <c r="F73" s="43" t="s">
+      <c r="F73" s="37" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4318,9 +4381,9 @@
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
-      </c>
-      <c r="C74" s="67">
+        <v>205</v>
+      </c>
+      <c r="C74" s="61">
         <v>198</v>
       </c>
       <c r="D74" t="s">
@@ -4338,9 +4401,9 @@
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="67">
+        <v>205</v>
+      </c>
+      <c r="C75" s="61">
         <v>198</v>
       </c>
       <c r="D75" t="s">
@@ -4354,42 +4417,42 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="43">
+      <c r="A76" s="37">
         <v>74</v>
       </c>
-      <c r="B76" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="44">
+      <c r="B76" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" s="38">
         <v>199</v>
       </c>
-      <c r="D76" s="43" t="s">
+      <c r="D76" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="E76" s="43">
+      <c r="E76" s="37">
         <v>310038031</v>
       </c>
-      <c r="F76" s="43" t="s">
+      <c r="F76" s="37" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="43">
+      <c r="A77" s="37">
         <v>76</v>
       </c>
-      <c r="B77" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77" s="44">
+      <c r="B77" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="38">
         <v>200</v>
       </c>
-      <c r="D77" s="43" t="s">
+      <c r="D77" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="E77" s="43">
+      <c r="E77" s="37">
         <v>310038031</v>
       </c>
-      <c r="F77" s="43" t="s">
+      <c r="F77" s="37" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4398,9 +4461,9 @@
         <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" s="67">
+        <v>207</v>
+      </c>
+      <c r="C78" s="61">
         <v>200</v>
       </c>
       <c r="D78" t="s">
@@ -4476,9 +4539,711 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2">
+        <v>132</v>
+      </c>
+      <c r="D2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3">
+        <v>135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5">
+        <v>139</v>
+      </c>
+      <c r="D5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8">
+        <v>144</v>
+      </c>
+      <c r="D8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9">
+        <v>225</v>
+      </c>
+      <c r="D9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10">
+        <v>228</v>
+      </c>
+      <c r="D10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11">
+        <v>229</v>
+      </c>
+      <c r="D11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12">
+        <v>231</v>
+      </c>
+      <c r="D12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C13">
+        <v>301</v>
+      </c>
+      <c r="D13" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14">
+        <v>304</v>
+      </c>
+      <c r="D14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15">
+        <v>307</v>
+      </c>
+      <c r="D15" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16">
+        <v>310</v>
+      </c>
+      <c r="D16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17">
+        <v>313</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18">
+        <v>316</v>
+      </c>
+      <c r="D18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19">
+        <v>319</v>
+      </c>
+      <c r="D19" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20">
+        <v>322</v>
+      </c>
+      <c r="D20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21">
+        <v>420</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22">
+        <v>421</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23">
+        <v>423</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" t="s">
+        <v>189</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24">
+        <v>424</v>
+      </c>
+      <c r="D24" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C25">
+        <v>503</v>
+      </c>
+      <c r="D25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26">
+        <v>506</v>
+      </c>
+      <c r="D26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27">
+        <v>509</v>
+      </c>
+      <c r="D27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28">
+        <v>512</v>
+      </c>
+      <c r="D28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29">
+        <v>515</v>
+      </c>
+      <c r="D29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30">
+        <v>503</v>
+      </c>
+      <c r="D30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30" t="s">
+        <v>196</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31">
+        <v>9189</v>
+      </c>
+      <c r="D31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32">
+        <v>9190</v>
+      </c>
+      <c r="D32" t="s">
+        <v>210</v>
+      </c>
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>208</v>
+      </c>
+      <c r="C33">
+        <v>9191</v>
+      </c>
+      <c r="D33" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33" t="s">
+        <v>199</v>
+      </c>
+      <c r="F33" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34">
+        <v>9192</v>
+      </c>
+      <c r="D34" t="s">
+        <v>210</v>
+      </c>
+      <c r="E34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C35">
+        <v>9193</v>
+      </c>
+      <c r="D35" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36">
+        <v>195</v>
+      </c>
+      <c r="D36" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" t="s">
+        <v>202</v>
+      </c>
+      <c r="F36" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37">
+        <v>196</v>
+      </c>
+      <c r="D37" t="s">
+        <v>210</v>
+      </c>
+      <c r="E37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38">
+        <v>197</v>
+      </c>
+      <c r="D38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E38" t="s">
+        <v>204</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C39">
+        <v>198</v>
+      </c>
+      <c r="D39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39" t="s">
+        <v>205</v>
+      </c>
+      <c r="F39" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>208</v>
+      </c>
+      <c r="C40">
+        <v>199</v>
+      </c>
+      <c r="D40" t="s">
+        <v>210</v>
+      </c>
+      <c r="E40" t="s">
+        <v>206</v>
+      </c>
+      <c r="F40" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41">
+        <v>200</v>
+      </c>
+      <c r="D41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" s="68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
@@ -5488,7 +6253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E79"/>
   <sheetViews>

</xml_diff>